<commit_message>
Updated oc-sonic mapping png
</commit_message>
<xml_diff>
--- a/doc/mgmt/Openconfig-system_SONiC_mapping.xlsx
+++ b/doc/mgmt/Openconfig-system_SONiC_mapping.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anukul/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anukul/Desktop/SONiC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA58B53C-5B85-F04D-870B-F4C72A153465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0C5603-5422-424A-813D-BA76CCF401AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="3220" windowWidth="28040" windowHeight="17440" xr2:uid="{81CB7C93-0B4F-8B49-B65D-B3FAC13D3449}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{81CB7C93-0B4F-8B49-B65D-B3FAC13D3449}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rev 0.1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="134">
   <si>
     <t>Openconfig Yang</t>
   </si>
@@ -86,12 +86,6 @@
     <t xml:space="preserve">              admin_state</t>
   </si>
   <si>
-    <t xml:space="preserve">    ntp-source-address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               vrf  &amp; src_intf</t>
-  </si>
-  <si>
     <t xml:space="preserve">    enable-ntp-auth</t>
   </si>
   <si>
@@ -396,13 +390,61 @@
   </si>
   <si>
     <t xml:space="preserve">     service</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>VERSION|SOFTWARE</t>
+  </si>
+  <si>
+    <t>BANNER_MESSAGE:login</t>
+  </si>
+  <si>
+    <t>BANNER_MESSAGE:motd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  login-banner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  motd-banner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  current-datatime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  up-time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  boot-time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  software-version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          network-instance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    vrf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          key-id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          NTP|global  vrf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          NTP|global  src_intf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -411,33 +453,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="16"/>
       <color rgb="FF3B3B3B"/>
-      <name val="Menlo"/>
-      <family val="2"/>
+      <name val="Times New Roman Bold"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF3B3B3B"/>
-      <name val="Menlo"/>
-      <family val="2"/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman Bold"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman Bold"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -467,22 +516,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,667 +869,741 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74ECBB5C-9524-6641-88D0-35FCDDE5B859}">
-  <dimension ref="A1:B93"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D085E869-6FAE-2547-AA24-288A774513A0}">
+  <dimension ref="A1:B104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="22"/>
   <cols>
-    <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="1" max="1" width="37.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="B2" s="5"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B22" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B23" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B24" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="B26" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B27" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B28" s="5"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="B29" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="4"/>
-    </row>
-    <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="B30" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B31" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="B33" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="5"/>
-    </row>
-    <row r="26" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B34" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="B36" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="B37" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B38" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B39" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+    <row r="40" spans="1:2">
+      <c r="A40" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="4"/>
+      <c r="B43" s="5"/>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B44" s="5"/>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="5"/>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+      <c r="B46" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="4"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="4"/>
+      <c r="B47" s="5"/>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B48" s="5"/>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+      <c r="B49" s="5"/>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="4"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+      <c r="B50" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="4"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B51" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B52" s="5"/>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B53" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="4"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+    <row r="54" spans="1:2">
+      <c r="A54" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B54" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+    <row r="55" spans="1:2">
+      <c r="A55" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B56" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" s="4"/>
+      <c r="B57" s="5"/>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B58" s="5"/>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="8" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="4"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
+      <c r="B59" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B47" s="4"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B60" s="5"/>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="8" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
+      <c r="B61" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B49" s="4"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B62" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" s="5"/>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="8" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
+      <c r="B64" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="6" t="s">
+      <c r="B65" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B66" s="5"/>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B52" s="4"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="6" t="s">
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B54" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" s="4"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="6" t="s">
+      <c r="B68" s="5"/>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="6" t="s">
+      <c r="B69" s="5"/>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B57" s="4"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="6" t="s">
+      <c r="B70" s="5"/>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="4"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="6" t="s">
+      <c r="B71" s="5"/>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B59" s="4"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="6" t="s">
+      <c r="B72" s="5"/>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B60" s="4"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="6" t="s">
+      <c r="B73" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B61" s="4"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="6" t="s">
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B74" s="5"/>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="6" t="s">
+      <c r="B75" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B63" s="4"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="6" t="s">
+      <c r="B76" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B64" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="6" t="s">
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B77" s="5"/>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="8" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="6" t="s">
+      <c r="B78" s="5"/>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B66" s="4"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="6" t="s">
+      <c r="B79" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B67" s="4"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="6" t="s">
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B80" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="6" t="s">
+    <row r="81" spans="1:2">
+      <c r="A81" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B81" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
+    <row r="82" spans="1:2">
+      <c r="A82" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B82" s="5"/>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="8" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="6" t="s">
+      <c r="B83" s="5"/>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B71" s="4"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="6" t="s">
+      <c r="B84" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B72" s="4"/>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="6" t="s">
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B85" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
+    <row r="86" spans="1:2">
+      <c r="A86" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B86" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="6" t="s">
+    <row r="87" spans="1:2">
+      <c r="A87" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B87" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="6" t="s">
+    <row r="88" spans="1:2">
+      <c r="A88" s="8"/>
+      <c r="B88" s="5"/>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B89" s="5"/>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="8" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="6"/>
-      <c r="B77" s="4"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="6" t="s">
+      <c r="B90" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B78" s="4"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="6" t="s">
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B91" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="6" t="s">
+    <row r="92" spans="1:2">
+      <c r="A92" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B92" s="5"/>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="6" t="s">
+      <c r="B93" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B94" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B81" s="4"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="6" t="s">
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B82" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B83" s="4" t="s">
+      <c r="B95" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="6" t="s">
+      <c r="B96" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B84" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="6" t="s">
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B97" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="6" t="s">
+    <row r="98" spans="1:2">
+      <c r="A98" s="8"/>
+      <c r="B98" s="5"/>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B99" s="5"/>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="8" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="6"/>
-      <c r="B87" s="4"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="6" t="s">
+      <c r="B100" s="5"/>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B88" s="4"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="6" t="s">
+      <c r="B101" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B89" s="4"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="6" t="s">
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B102" s="5"/>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="8" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="6" t="s">
+      <c r="B103" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B91" s="4"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="6" t="s">
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B104" s="5" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;R_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Cisco Confidential</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>